<commit_message>
7월 2~3주차 계획 commit
</commit_message>
<xml_diff>
--- a/SourceCode/개발 일정표.xlsx
+++ b/SourceCode/개발 일정표.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HIG\Desktop\GGCS\SourceCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seongho Chun\Documents\GGCS\SourceCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE81569B-43AC-495B-BDB3-E4CD6AEEA3BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485AE47-791E-433F-AE01-1C72A00AB4B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>7월</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,6 +118,14 @@
     <t xml:space="preserve">1. 안드로이드 앱에서 미구현된 화면들이 포함할 세부 기능들 설계 및 정리
 2. 1번의 설계 사항에 맞춰 앱 구현
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터 기능 구현 및 webOS 개발을 위한 환경 설정(Ubuntu 설치 및 webOS emulator 설치)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼 입력 받기, 식사 기능 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,18 +437,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -449,20 +448,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -745,252 +753,256 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="7" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="21" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
-    <row r="2" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="70.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:15" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="10"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="11"/>
+      <c r="K4" s="8"/>
       <c r="L4" s="2"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="11"/>
+      <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="11"/>
+      <c r="K5" s="8"/>
       <c r="L5" s="2"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="11"/>
+      <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="11"/>
+      <c r="K6" s="8"/>
       <c r="L6" s="2"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="11"/>
+      <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="11"/>
+      <c r="K7" s="8"/>
       <c r="L7" s="2"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="11"/>
+      <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="11"/>
+      <c r="K8" s="8"/>
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="11"/>
+      <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="24"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="11"/>
+      <c r="K9" s="8"/>
       <c r="L9" s="2"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="11"/>
+      <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>